<commit_message>
solved min swap to sort
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A70FBE2-5563-42A3-947F-0CE05388BA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC4CD37-515C-4DA7-8D30-C37908A6398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="524">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1479,24 +1479,12 @@
     <t>*ternary Search Later</t>
   </si>
   <si>
-    <t>*graph</t>
-  </si>
-  <si>
     <t>*later</t>
   </si>
   <si>
     <t>Theory</t>
   </si>
   <si>
-    <t>*heap</t>
-  </si>
-  <si>
-    <t>Also Do Sort Nearly Sorted Array Or K Sorted Array</t>
-  </si>
-  <si>
-    <t>*Do It Later</t>
-  </si>
-  <si>
     <t>*Queue &amp; Hash</t>
   </si>
   <si>
@@ -1606,6 +1594,18 @@
   </si>
   <si>
     <t>Kind Of Dp</t>
+  </si>
+  <si>
+    <t>inbuilt stable_sort() or use bucket sort</t>
+  </si>
+  <si>
+    <t>Possible In Case Of Doubly Linked List Swaping The Tail And Head Pointer</t>
+  </si>
+  <si>
+    <t>DLL</t>
+  </si>
+  <si>
+    <t>*Do It Later DLL</t>
   </si>
 </sst>
 </file>
@@ -2077,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2265,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>456</v>
@@ -2540,7 +2540,7 @@
         <v>5</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>456</v>
@@ -2551,7 +2551,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>456</v>
@@ -2639,7 +2639,7 @@
         <v>456</v>
       </c>
       <c r="D52" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="21">
@@ -2686,7 +2686,7 @@
         <v>456</v>
       </c>
       <c r="D56" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="19.5">
@@ -2694,7 +2694,7 @@
         <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>456</v>
@@ -2746,7 +2746,7 @@
         <v>54</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="21">
@@ -2801,7 +2801,7 @@
         <v>50</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>4</v>
@@ -3082,7 +3082,7 @@
         <v>4</v>
       </c>
       <c r="D89" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="21">
@@ -3124,7 +3124,7 @@
         <v>456</v>
       </c>
       <c r="D92" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="21">
@@ -3163,7 +3163,7 @@
         <v>456</v>
       </c>
       <c r="D95" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="21">
@@ -3384,7 +3384,7 @@
         <v>103</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="21">
@@ -3395,10 +3395,7 @@
         <v>104</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D116" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="21">
@@ -3453,10 +3450,10 @@
         <v>109</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
       <c r="D121" t="s">
-        <v>479</v>
+        <v>520</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="21">
@@ -3467,10 +3464,7 @@
         <v>110</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D122" t="s">
-        <v>481</v>
+        <v>456</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="21">
@@ -3495,7 +3489,7 @@
         <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="21">
@@ -3572,10 +3566,7 @@
         <v>119</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D131" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="21">
@@ -3633,7 +3624,7 @@
         <v>4</v>
       </c>
       <c r="D136" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -3644,10 +3635,7 @@
         <v>125</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D137" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -3683,7 +3671,7 @@
         <v>128</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -3893,7 +3881,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="21">
+    <row r="161" spans="1:4" ht="21">
       <c r="A161" s="8" t="s">
         <v>129</v>
       </c>
@@ -3904,7 +3892,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="21">
+    <row r="162" spans="1:4" ht="21">
       <c r="A162" s="8" t="s">
         <v>129</v>
       </c>
@@ -3915,7 +3903,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="21">
+    <row r="163" spans="1:4" ht="21">
       <c r="A163" s="8" t="s">
         <v>129</v>
       </c>
@@ -3926,7 +3914,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="21">
+    <row r="164" spans="1:4" ht="21">
       <c r="A164" s="8" t="s">
         <v>129</v>
       </c>
@@ -3937,7 +3925,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="21">
+    <row r="165" spans="1:4" ht="21">
       <c r="A165" s="8" t="s">
         <v>129</v>
       </c>
@@ -3948,7 +3936,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="21">
+    <row r="166" spans="1:4" ht="21">
       <c r="A166" s="8" t="s">
         <v>129</v>
       </c>
@@ -3956,16 +3944,10 @@
         <v>152</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D166" t="s">
-        <v>484</v>
-      </c>
-      <c r="E166" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="21">
       <c r="A167" s="8" t="s">
         <v>129</v>
       </c>
@@ -3976,7 +3958,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="21">
+    <row r="168" spans="1:4" ht="21">
       <c r="A168" s="8" t="s">
         <v>129</v>
       </c>
@@ -3987,10 +3969,10 @@
         <v>4</v>
       </c>
       <c r="D168" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="21">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="21">
       <c r="A169" s="8" t="s">
         <v>129</v>
       </c>
@@ -4000,8 +3982,11 @@
       <c r="C169" s="4" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" ht="21">
+      <c r="D169" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="21">
       <c r="A170" s="8" t="s">
         <v>129</v>
       </c>
@@ -4012,7 +3997,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="21">
+    <row r="171" spans="1:4" ht="21">
       <c r="A171" s="8" t="s">
         <v>129</v>
       </c>
@@ -4023,7 +4008,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="21">
+    <row r="172" spans="1:4" ht="21">
       <c r="A172" s="8" t="s">
         <v>129</v>
       </c>
@@ -4034,7 +4019,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="21">
+    <row r="173" spans="1:4" ht="21">
       <c r="A173" s="8" t="s">
         <v>129</v>
       </c>
@@ -4045,7 +4030,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="21">
+    <row r="174" spans="1:4" ht="21">
       <c r="A174" s="8" t="s">
         <v>129</v>
       </c>
@@ -4053,10 +4038,10 @@
         <v>160</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="21">
       <c r="A175" s="8" t="s">
         <v>129</v>
       </c>
@@ -4067,7 +4052,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="21">
+    <row r="176" spans="1:4" ht="21">
       <c r="A176" s="8" t="s">
         <v>129</v>
       </c>
@@ -4111,7 +4096,7 @@
         <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="21">
@@ -4119,7 +4104,7 @@
         <v>129</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>456</v>
@@ -4130,7 +4115,7 @@
         <v>129</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>4</v>
@@ -4141,10 +4126,13 @@
         <v>129</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="D182" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="21">
@@ -4152,10 +4140,13 @@
         <v>129</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="D183" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">
@@ -4426,7 +4417,7 @@
         <v>456</v>
       </c>
       <c r="D208" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4440,7 +4431,7 @@
         <v>4</v>
       </c>
       <c r="D209" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="21">
@@ -4558,7 +4549,7 @@
         <v>166</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>4</v>
@@ -4888,7 +4879,7 @@
         <v>4</v>
       </c>
       <c r="D252" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="21">
@@ -4896,7 +4887,7 @@
         <v>225</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>456</v>
@@ -5122,7 +5113,7 @@
         <v>4</v>
       </c>
       <c r="D273" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="21">
@@ -5180,7 +5171,7 @@
         <v>4</v>
       </c>
       <c r="D278" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="21">
@@ -5323,7 +5314,7 @@
         <v>4</v>
       </c>
       <c r="D292" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="21">
@@ -5430,7 +5421,7 @@
         <v>259</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C302" s="4" t="s">
         <v>4</v>
@@ -5499,10 +5490,10 @@
         <v>456</v>
       </c>
       <c r="D309" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="E309" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="310" spans="1:5" ht="21">
@@ -5582,7 +5573,7 @@
         <v>456</v>
       </c>
       <c r="D316" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="317" spans="1:5" ht="21">
@@ -5808,10 +5799,10 @@
         <v>4</v>
       </c>
       <c r="D336" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E336" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="21">
@@ -5825,7 +5816,7 @@
         <v>4</v>
       </c>
       <c r="D337" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="21">
@@ -5850,7 +5841,7 @@
         <v>4</v>
       </c>
       <c r="D339" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="21">
@@ -5908,7 +5899,7 @@
         <v>278</v>
       </c>
       <c r="B344" s="6" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C344" s="4" t="s">
         <v>4</v>
@@ -5919,7 +5910,7 @@
         <v>278</v>
       </c>
       <c r="B345" s="6" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C345" s="4" t="s">
         <v>4</v>
@@ -5934,7 +5925,7 @@
         <v>317</v>
       </c>
       <c r="B347" s="7" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C347" s="4" t="s">
         <v>456</v>
@@ -6399,7 +6390,7 @@
         <v>4</v>
       </c>
       <c r="D390" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="21">
@@ -6413,7 +6404,7 @@
         <v>456</v>
       </c>
       <c r="D391" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="392" spans="1:4" ht="21">
@@ -6424,7 +6415,7 @@
         <v>361</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="393" spans="1:4" ht="21">
@@ -6740,7 +6731,7 @@
         <v>456</v>
       </c>
       <c r="D423" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="21">
@@ -6836,7 +6827,7 @@
         <v>385</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>456</v>
@@ -7494,7 +7485,7 @@
         <v>444</v>
       </c>
       <c r="B493" s="6" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C493" s="4" t="s">
         <v>456</v>

</xml_diff>

<commit_message>
solved some tree porblems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC4CD37-515C-4DA7-8D30-C37908A6398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A430EBB-71D8-49E6-AEED-A255AC3C4923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="527">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1606,6 +1606,15 @@
   </si>
   <si>
     <t>*Do It Later DLL</t>
+  </si>
+  <si>
+    <t>Break down to min swap req to sort an array</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for cycle and all the compoenets are connected </t>
   </si>
 </sst>
 </file>
@@ -2077,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3466,6 +3475,9 @@
       <c r="C122" s="4" t="s">
         <v>456</v>
       </c>
+      <c r="D122" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="123" spans="1:4" ht="21">
       <c r="A123" s="5" t="s">
@@ -4337,7 +4349,7 @@
         <v>183</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="21">
@@ -4381,7 +4393,10 @@
         <v>187</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
+      </c>
+      <c r="D205" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="21">
@@ -4442,7 +4457,7 @@
         <v>192</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="21">
@@ -4453,7 +4468,10 @@
         <v>193</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
+      </c>
+      <c r="D211" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -4464,7 +4482,7 @@
         <v>194</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -4475,7 +4493,7 @@
         <v>195</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="21">

</xml_diff>

<commit_message>
solved path sum 3 and camera bt
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A430EBB-71D8-49E6-AEED-A255AC3C4923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6DF1A2-463A-4563-8C4B-FF93F94ED580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1615,6 +1615,12 @@
   </si>
   <si>
     <t xml:space="preserve">Check for cycle and all the compoenets are connected </t>
+  </si>
+  <si>
+    <t>Cameras On Binary Tree</t>
+  </si>
+  <si>
+    <t>Morris Inorder Traversal</t>
   </si>
 </sst>
 </file>
@@ -2084,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F493"/>
+  <dimension ref="A1:F494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A276" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4504,7 +4510,7 @@
         <v>196</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="21">
@@ -4574,9 +4580,15 @@
       </c>
     </row>
     <row r="221" spans="1:4" ht="21">
-      <c r="A221" s="8"/>
-      <c r="B221" s="7"/>
-      <c r="C221" s="4"/>
+      <c r="A221" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="222" spans="1:4" ht="21">
       <c r="A222" s="8"/>
@@ -4584,201 +4596,198 @@
       <c r="C222" s="4"/>
     </row>
     <row r="223" spans="1:4" ht="21">
-      <c r="A223" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B223" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C223" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="A223" s="8"/>
+      <c r="B223" s="7"/>
+      <c r="C223" s="4"/>
     </row>
     <row r="224" spans="1:4" ht="21">
       <c r="A224" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="21">
+    <row r="225" spans="1:4" ht="21">
       <c r="A225" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="21">
+    <row r="226" spans="1:4" ht="21">
       <c r="A226" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="21">
+    <row r="227" spans="1:4" ht="21">
       <c r="A227" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="21">
+    <row r="228" spans="1:4" ht="21">
       <c r="A228" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="21">
+    <row r="229" spans="1:4" ht="21">
       <c r="A229" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B229" s="9" t="s">
-        <v>209</v>
+      <c r="B229" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="21">
+    <row r="230" spans="1:4" ht="21">
       <c r="A230" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B230" s="6" t="s">
-        <v>210</v>
+      <c r="B230" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="21">
+    <row r="231" spans="1:4" ht="21">
       <c r="A231" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="21">
+    <row r="232" spans="1:4" ht="21">
       <c r="A232" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="21">
+    <row r="233" spans="1:4" ht="21">
       <c r="A233" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="21">
+    <row r="234" spans="1:4" ht="21">
       <c r="A234" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="21">
+    <row r="235" spans="1:4" ht="21">
       <c r="A235" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="21">
+    <row r="236" spans="1:4" ht="21">
       <c r="A236" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="21">
+    <row r="237" spans="1:4" ht="21">
       <c r="A237" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="21">
       <c r="A238" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="21">
+        <v>4</v>
+      </c>
+      <c r="D238" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="21">
       <c r="A239" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="21">
+    <row r="240" spans="1:4" ht="21">
       <c r="A240" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="21">
@@ -4786,10 +4795,10 @@
         <v>202</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="21">
@@ -4797,10 +4806,10 @@
         <v>202</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="21">
@@ -4808,10 +4817,10 @@
         <v>202</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="21">
@@ -4819,35 +4828,37 @@
         <v>202</v>
       </c>
       <c r="B244" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="21">
+      <c r="A245" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B245" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C244" s="4"/>
-    </row>
-    <row r="245" spans="1:4" ht="21">
-      <c r="B245" s="7"/>
-      <c r="C245" s="4"/>
+      <c r="C245" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="246" spans="1:4" ht="21">
       <c r="B246" s="7"/>
       <c r="C246" s="4"/>
     </row>
     <row r="247" spans="1:4" ht="21">
-      <c r="A247" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B247" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C247" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B247" s="7"/>
+      <c r="C247" s="4"/>
     </row>
     <row r="248" spans="1:4" ht="21">
       <c r="A248" s="5" t="s">
         <v>225</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>456</v>
@@ -4858,7 +4869,7 @@
         <v>225</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>456</v>
@@ -4869,7 +4880,7 @@
         <v>225</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>456</v>
@@ -4880,7 +4891,7 @@
         <v>225</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>456</v>
@@ -4891,13 +4902,10 @@
         <v>225</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D252" t="s">
-        <v>510</v>
+        <v>456</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="21">
@@ -4905,10 +4913,13 @@
         <v>225</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>513</v>
+        <v>231</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
+      </c>
+      <c r="D253" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="21">
@@ -4916,7 +4927,7 @@
         <v>225</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>232</v>
+        <v>513</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>456</v>
@@ -4927,7 +4938,7 @@
         <v>225</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>456</v>
@@ -4938,7 +4949,7 @@
         <v>225</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>456</v>
@@ -4949,7 +4960,7 @@
         <v>225</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>456</v>
@@ -4960,7 +4971,7 @@
         <v>225</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>456</v>
@@ -4971,7 +4982,7 @@
         <v>225</v>
       </c>
       <c r="B259" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>456</v>
@@ -4982,7 +4993,7 @@
         <v>225</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>456</v>
@@ -4993,7 +5004,7 @@
         <v>225</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>456</v>
@@ -5004,7 +5015,7 @@
         <v>225</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>456</v>
@@ -5015,7 +5026,7 @@
         <v>225</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>456</v>
@@ -5026,7 +5037,7 @@
         <v>225</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>456</v>
@@ -5037,7 +5048,7 @@
         <v>225</v>
       </c>
       <c r="B265" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>456</v>
@@ -5048,7 +5059,7 @@
         <v>225</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>456</v>
@@ -5059,7 +5070,7 @@
         <v>225</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>456</v>
@@ -5070,7 +5081,7 @@
         <v>225</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>456</v>
@@ -5092,7 +5103,7 @@
         <v>225</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>456</v>
@@ -5103,7 +5114,7 @@
         <v>225</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>456</v>
@@ -5114,7 +5125,7 @@
         <v>225</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>456</v>
@@ -5125,13 +5136,10 @@
         <v>225</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D273" t="s">
-        <v>510</v>
+        <v>456</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="21">
@@ -5139,10 +5147,13 @@
         <v>225</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
+      </c>
+      <c r="D274" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="21">
@@ -5150,7 +5161,7 @@
         <v>225</v>
       </c>
       <c r="B275" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>456</v>
@@ -5161,7 +5172,7 @@
         <v>225</v>
       </c>
       <c r="B276" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>456</v>
@@ -5172,7 +5183,7 @@
         <v>225</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>456</v>
@@ -5183,13 +5194,10 @@
         <v>225</v>
       </c>
       <c r="B278" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D278" t="s">
-        <v>514</v>
+        <v>456</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="21">
@@ -5197,10 +5205,13 @@
         <v>225</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
+      </c>
+      <c r="D279" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="21">
@@ -5208,7 +5219,7 @@
         <v>225</v>
       </c>
       <c r="B280" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>456</v>
@@ -5219,7 +5230,7 @@
         <v>225</v>
       </c>
       <c r="B281" s="6" t="s">
-        <v>82</v>
+        <v>257</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>456</v>
@@ -5230,37 +5241,37 @@
         <v>225</v>
       </c>
       <c r="B282" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C282" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="21">
+      <c r="A283" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B283" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C282" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4" ht="21">
-      <c r="B283" s="7"/>
-      <c r="C283" s="4"/>
+      <c r="C283" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="284" spans="1:4" ht="21">
       <c r="B284" s="7"/>
       <c r="C284" s="4"/>
     </row>
     <row r="285" spans="1:4" ht="21">
-      <c r="A285" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B285" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C285" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B285" s="7"/>
+      <c r="C285" s="4"/>
     </row>
     <row r="286" spans="1:4" ht="21">
       <c r="A286" s="5" t="s">
         <v>259</v>
       </c>
       <c r="B286" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>456</v>
@@ -5271,7 +5282,7 @@
         <v>259</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>456</v>
@@ -5282,7 +5293,7 @@
         <v>259</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C288" s="4" t="s">
         <v>456</v>
@@ -5293,7 +5304,7 @@
         <v>259</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C289" s="4" t="s">
         <v>456</v>
@@ -5304,7 +5315,7 @@
         <v>259</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C290" s="4" t="s">
         <v>456</v>
@@ -5315,7 +5326,7 @@
         <v>259</v>
       </c>
       <c r="B291" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C291" s="4" t="s">
         <v>456</v>
@@ -5326,13 +5337,10 @@
         <v>259</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D292" t="s">
-        <v>510</v>
+        <v>456</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="21">
@@ -5340,10 +5348,13 @@
         <v>259</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
+      </c>
+      <c r="D293" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="21">
@@ -5351,7 +5362,7 @@
         <v>259</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>456</v>
@@ -5362,7 +5373,7 @@
         <v>259</v>
       </c>
       <c r="B295" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C295" s="4" t="s">
         <v>456</v>
@@ -5373,7 +5384,7 @@
         <v>259</v>
       </c>
       <c r="B296" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C296" s="4" t="s">
         <v>456</v>
@@ -5384,7 +5395,7 @@
         <v>259</v>
       </c>
       <c r="B297" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C297" s="4" t="s">
         <v>456</v>
@@ -5395,7 +5406,7 @@
         <v>259</v>
       </c>
       <c r="B298" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C298" s="4" t="s">
         <v>456</v>
@@ -5406,7 +5417,7 @@
         <v>259</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C299" s="4" t="s">
         <v>456</v>
@@ -5417,7 +5428,7 @@
         <v>259</v>
       </c>
       <c r="B300" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C300" s="4" t="s">
         <v>456</v>
@@ -5428,7 +5439,7 @@
         <v>259</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C301" s="4" t="s">
         <v>456</v>
@@ -5439,10 +5450,10 @@
         <v>259</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>515</v>
+        <v>276</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="21">
@@ -5450,37 +5461,37 @@
         <v>259</v>
       </c>
       <c r="B303" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" ht="21">
+      <c r="A304" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B304" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C303" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4" ht="21">
-      <c r="B304" s="7"/>
-      <c r="C304" s="4"/>
+      <c r="C304" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="305" spans="1:5" ht="21">
       <c r="B305" s="7"/>
       <c r="C305" s="4"/>
     </row>
     <row r="306" spans="1:5" ht="21">
-      <c r="A306" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B306" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C306" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B306" s="7"/>
+      <c r="C306" s="4"/>
     </row>
     <row r="307" spans="1:5" ht="21">
       <c r="A307" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C307" s="4" t="s">
         <v>456</v>
@@ -5491,7 +5502,7 @@
         <v>278</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C308" s="4" t="s">
         <v>456</v>
@@ -5502,16 +5513,10 @@
         <v>278</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C309" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="D309" t="s">
-        <v>488</v>
-      </c>
-      <c r="E309" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="310" spans="1:5" ht="21">
@@ -5519,10 +5524,16 @@
         <v>278</v>
       </c>
       <c r="B310" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C310" s="4" t="s">
         <v>456</v>
+      </c>
+      <c r="D310" t="s">
+        <v>488</v>
+      </c>
+      <c r="E310" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="311" spans="1:5" ht="21">
@@ -5530,7 +5541,7 @@
         <v>278</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C311" s="4" t="s">
         <v>456</v>
@@ -5541,7 +5552,7 @@
         <v>278</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C312" s="4" t="s">
         <v>456</v>
@@ -5552,7 +5563,7 @@
         <v>278</v>
       </c>
       <c r="B313" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>456</v>
@@ -5563,7 +5574,7 @@
         <v>278</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>456</v>
@@ -5574,7 +5585,7 @@
         <v>278</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C315" s="4" t="s">
         <v>456</v>
@@ -5585,13 +5596,10 @@
         <v>278</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="D316" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="317" spans="1:5" ht="21">
@@ -5599,10 +5607,13 @@
         <v>278</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>456</v>
+      </c>
+      <c r="D317" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="318" spans="1:5" ht="21">
@@ -5610,7 +5621,7 @@
         <v>278</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C318" s="4" t="s">
         <v>456</v>
@@ -5620,8 +5631,8 @@
       <c r="A319" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B319" s="9" t="s">
-        <v>292</v>
+      <c r="B319" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="C319" s="4" t="s">
         <v>456</v>
@@ -5631,374 +5642,374 @@
       <c r="A320" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B320" s="6" t="s">
-        <v>293</v>
+      <c r="B320" s="9" t="s">
+        <v>292</v>
       </c>
       <c r="C320" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="321" spans="1:5" ht="21">
+    <row r="321" spans="1:4" ht="21">
       <c r="A321" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B321" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C321" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="322" spans="1:5" ht="21">
+    <row r="322" spans="1:4" ht="21">
       <c r="A322" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B322" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C322" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="323" spans="1:5" ht="21">
+    <row r="323" spans="1:4" ht="21">
       <c r="A323" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C323" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="324" spans="1:5" ht="21">
+    <row r="324" spans="1:4" ht="21">
       <c r="A324" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B324" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C324" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="325" spans="1:5" ht="21">
+    <row r="325" spans="1:4" ht="21">
       <c r="A325" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C325" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="326" spans="1:5" ht="21">
+    <row r="326" spans="1:4" ht="21">
       <c r="A326" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C326" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="327" spans="1:5" ht="21">
+    <row r="327" spans="1:4" ht="21">
       <c r="A327" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C327" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="328" spans="1:5" ht="21">
+    <row r="328" spans="1:4" ht="21">
       <c r="A328" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B328" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C328" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="329" spans="1:5" ht="21">
+    <row r="329" spans="1:4" ht="21">
       <c r="A329" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="330" spans="1:5" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" ht="21">
       <c r="A330" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="331" spans="1:5" ht="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" ht="21">
       <c r="A331" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D331" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="332" spans="1:5" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" ht="21">
       <c r="A332" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="333" spans="1:5" ht="21">
+        <v>4</v>
+      </c>
+      <c r="D332" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" ht="21">
       <c r="A333" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C333" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="334" spans="1:5" ht="21">
+    <row r="334" spans="1:4" ht="21">
       <c r="A334" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C334" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="335" spans="1:5" ht="21">
+    <row r="335" spans="1:4" ht="21">
       <c r="A335" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C335" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="336" spans="1:5" ht="21">
+    <row r="336" spans="1:4" ht="21">
       <c r="A336" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D336" t="s">
-        <v>492</v>
-      </c>
-      <c r="E336" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="337" spans="1:4" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" ht="21">
       <c r="A337" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C337" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D337" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="338" spans="1:4" ht="21">
+        <v>492</v>
+      </c>
+      <c r="E337" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" ht="21">
       <c r="A338" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B338" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" ht="21">
+        <v>4</v>
+      </c>
+      <c r="D338" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" ht="21">
       <c r="A339" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B339" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D339" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" ht="21">
       <c r="A340" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B340" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" ht="21">
+        <v>4</v>
+      </c>
+      <c r="D340" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" ht="21">
       <c r="A341" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B341" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D341" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" ht="21">
       <c r="A342" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B342" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C342" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D342" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" ht="21">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" ht="21">
       <c r="A343" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B343" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" ht="21">
+        <v>4</v>
+      </c>
+      <c r="D343" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" ht="21">
       <c r="A344" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B344" s="6" t="s">
-        <v>496</v>
+        <v>316</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" ht="21">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" ht="21">
       <c r="A345" s="5" t="s">
         <v>278</v>
       </c>
       <c r="B345" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C345" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="21">
-      <c r="B346" s="7"/>
-      <c r="C346" s="4"/>
-    </row>
-    <row r="347" spans="1:4" ht="21">
-      <c r="A347" s="5" t="s">
+    <row r="346" spans="1:5" ht="21">
+      <c r="A346" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="C346" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" ht="21">
+      <c r="B347" s="7"/>
+      <c r="C347" s="4"/>
+    </row>
+    <row r="348" spans="1:5" ht="21">
+      <c r="A348" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B347" s="7" t="s">
+      <c r="B348" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="C347" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="348" spans="1:4" ht="21">
-      <c r="A348" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B348" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="C348" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="349" spans="1:4" ht="21">
+    <row r="349" spans="1:5" ht="21">
       <c r="A349" s="8" t="s">
         <v>317</v>
       </c>
       <c r="B349" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C349" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="350" spans="1:4" ht="21">
+    <row r="350" spans="1:5" ht="21">
       <c r="A350" s="8" t="s">
         <v>317</v>
       </c>
       <c r="B350" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C350" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="21">
+    <row r="351" spans="1:5" ht="21">
       <c r="A351" s="8" t="s">
         <v>317</v>
       </c>
       <c r="B351" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C351" s="4" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="21">
+    <row r="352" spans="1:5" ht="21">
       <c r="A352" s="8" t="s">
         <v>317</v>
       </c>
       <c r="B352" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C352" s="4" t="s">
         <v>456</v>
@@ -6009,7 +6020,7 @@
         <v>317</v>
       </c>
       <c r="B353" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C353" s="4" t="s">
         <v>456</v>
@@ -6020,7 +6031,7 @@
         <v>317</v>
       </c>
       <c r="B354" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C354" s="4" t="s">
         <v>456</v>
@@ -6031,7 +6042,7 @@
         <v>317</v>
       </c>
       <c r="B355" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C355" s="4" t="s">
         <v>456</v>
@@ -6041,8 +6052,8 @@
       <c r="A356" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B356" s="9" t="s">
-        <v>326</v>
+      <c r="B356" s="6" t="s">
+        <v>325</v>
       </c>
       <c r="C356" s="4" t="s">
         <v>456</v>
@@ -6052,8 +6063,8 @@
       <c r="A357" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B357" s="6" t="s">
-        <v>327</v>
+      <c r="B357" s="9" t="s">
+        <v>326</v>
       </c>
       <c r="C357" s="4" t="s">
         <v>456</v>
@@ -6064,10 +6075,10 @@
         <v>317</v>
       </c>
       <c r="B358" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -6075,10 +6086,10 @@
         <v>317</v>
       </c>
       <c r="B359" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">
@@ -6086,7 +6097,7 @@
         <v>317</v>
       </c>
       <c r="B360" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C360" s="4" t="s">
         <v>456</v>
@@ -6097,7 +6108,7 @@
         <v>317</v>
       </c>
       <c r="B361" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C361" s="4" t="s">
         <v>456</v>
@@ -6108,7 +6119,7 @@
         <v>317</v>
       </c>
       <c r="B362" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C362" s="4" t="s">
         <v>456</v>
@@ -6119,7 +6130,7 @@
         <v>317</v>
       </c>
       <c r="B363" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C363" s="4" t="s">
         <v>456</v>
@@ -6130,7 +6141,7 @@
         <v>317</v>
       </c>
       <c r="B364" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C364" s="4" t="s">
         <v>456</v>
@@ -6141,37 +6152,37 @@
         <v>317</v>
       </c>
       <c r="B365" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C365" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" ht="21">
+      <c r="A366" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B366" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="C365" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="366" spans="1:3" ht="21">
-      <c r="B366" s="7"/>
-      <c r="C366" s="4"/>
+      <c r="C366" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="B367" s="7"/>
       <c r="C367" s="4"/>
     </row>
     <row r="368" spans="1:3" ht="21">
-      <c r="A368" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="B368" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C368" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B368" s="7"/>
+      <c r="C368" s="4"/>
     </row>
     <row r="369" spans="1:3" ht="21">
       <c r="A369" s="8" t="s">
         <v>336</v>
       </c>
       <c r="B369" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C369" s="4" t="s">
         <v>456</v>
@@ -6182,7 +6193,7 @@
         <v>336</v>
       </c>
       <c r="B370" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C370" s="4" t="s">
         <v>456</v>
@@ -6193,7 +6204,7 @@
         <v>336</v>
       </c>
       <c r="B371" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C371" s="4" t="s">
         <v>456</v>
@@ -6204,7 +6215,7 @@
         <v>336</v>
       </c>
       <c r="B372" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C372" s="4" t="s">
         <v>456</v>
@@ -6215,7 +6226,7 @@
         <v>336</v>
       </c>
       <c r="B373" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C373" s="4" t="s">
         <v>456</v>
@@ -6226,7 +6237,7 @@
         <v>336</v>
       </c>
       <c r="B374" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C374" s="4" t="s">
         <v>456</v>
@@ -6237,7 +6248,7 @@
         <v>336</v>
       </c>
       <c r="B375" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C375" s="4" t="s">
         <v>456</v>
@@ -6248,7 +6259,7 @@
         <v>336</v>
       </c>
       <c r="B376" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C376" s="4" t="s">
         <v>456</v>
@@ -6259,7 +6270,7 @@
         <v>336</v>
       </c>
       <c r="B377" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C377" s="4" t="s">
         <v>456</v>
@@ -6270,7 +6281,7 @@
         <v>336</v>
       </c>
       <c r="B378" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C378" s="4" t="s">
         <v>456</v>
@@ -6281,7 +6292,7 @@
         <v>336</v>
       </c>
       <c r="B379" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C379" s="4" t="s">
         <v>456</v>
@@ -6292,7 +6303,7 @@
         <v>336</v>
       </c>
       <c r="B380" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C380" s="4" t="s">
         <v>456</v>
@@ -6303,7 +6314,7 @@
         <v>336</v>
       </c>
       <c r="B381" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C381" s="4" t="s">
         <v>456</v>
@@ -6314,7 +6325,7 @@
         <v>336</v>
       </c>
       <c r="B382" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C382" s="4" t="s">
         <v>456</v>
@@ -6325,7 +6336,7 @@
         <v>336</v>
       </c>
       <c r="B383" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C383" s="4" t="s">
         <v>456</v>
@@ -6336,7 +6347,7 @@
         <v>336</v>
       </c>
       <c r="B384" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C384" s="4" t="s">
         <v>456</v>
@@ -6347,7 +6358,7 @@
         <v>336</v>
       </c>
       <c r="B385" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C385" s="4" t="s">
         <v>456</v>
@@ -6358,7 +6369,7 @@
         <v>336</v>
       </c>
       <c r="B386" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C386" s="4" t="s">
         <v>456</v>
@@ -6369,7 +6380,7 @@
         <v>336</v>
       </c>
       <c r="B387" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C387" s="4" t="s">
         <v>456</v>
@@ -6380,7 +6391,7 @@
         <v>336</v>
       </c>
       <c r="B388" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C388" s="4" t="s">
         <v>456</v>
@@ -6391,7 +6402,7 @@
         <v>336</v>
       </c>
       <c r="B389" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C389" s="4" t="s">
         <v>456</v>
@@ -6402,13 +6413,10 @@
         <v>336</v>
       </c>
       <c r="B390" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D390" t="s">
-        <v>510</v>
+        <v>456</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="21">
@@ -6416,13 +6424,13 @@
         <v>336</v>
       </c>
       <c r="B391" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
       <c r="D391" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="392" spans="1:4" ht="21">
@@ -6430,10 +6438,13 @@
         <v>336</v>
       </c>
       <c r="B392" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>511</v>
+        <v>456</v>
+      </c>
+      <c r="D392" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="393" spans="1:4" ht="21">
@@ -6441,10 +6452,10 @@
         <v>336</v>
       </c>
       <c r="B393" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>456</v>
+        <v>511</v>
       </c>
     </row>
     <row r="394" spans="1:4" ht="21">
@@ -6452,7 +6463,7 @@
         <v>336</v>
       </c>
       <c r="B394" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C394" s="4" t="s">
         <v>456</v>
@@ -6463,7 +6474,7 @@
         <v>336</v>
       </c>
       <c r="B395" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C395" s="4" t="s">
         <v>456</v>
@@ -6474,7 +6485,7 @@
         <v>336</v>
       </c>
       <c r="B396" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C396" s="4" t="s">
         <v>456</v>
@@ -6485,7 +6496,7 @@
         <v>336</v>
       </c>
       <c r="B397" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C397" s="4" t="s">
         <v>456</v>
@@ -6496,7 +6507,7 @@
         <v>336</v>
       </c>
       <c r="B398" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C398" s="4" t="s">
         <v>456</v>
@@ -6507,7 +6518,7 @@
         <v>336</v>
       </c>
       <c r="B399" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C399" s="4" t="s">
         <v>456</v>
@@ -6518,7 +6529,7 @@
         <v>336</v>
       </c>
       <c r="B400" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C400" s="4" t="s">
         <v>456</v>
@@ -6529,7 +6540,7 @@
         <v>336</v>
       </c>
       <c r="B401" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C401" s="4" t="s">
         <v>456</v>
@@ -6540,7 +6551,7 @@
         <v>336</v>
       </c>
       <c r="B402" s="6" t="s">
-        <v>274</v>
+        <v>370</v>
       </c>
       <c r="C402" s="4" t="s">
         <v>456</v>
@@ -6551,7 +6562,7 @@
         <v>336</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>371</v>
+        <v>274</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>456</v>
@@ -6562,7 +6573,7 @@
         <v>336</v>
       </c>
       <c r="B404" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C404" s="4" t="s">
         <v>456</v>
@@ -6573,7 +6584,7 @@
         <v>336</v>
       </c>
       <c r="B405" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C405" s="4" t="s">
         <v>456</v>
@@ -6584,10 +6595,10 @@
         <v>336</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">
@@ -6595,7 +6606,7 @@
         <v>336</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C407" s="4" t="s">
         <v>4</v>
@@ -6606,10 +6617,10 @@
         <v>336</v>
       </c>
       <c r="B408" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C408" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">
@@ -6617,7 +6628,7 @@
         <v>336</v>
       </c>
       <c r="B409" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C409" s="4" t="s">
         <v>456</v>
@@ -6628,40 +6639,40 @@
         <v>336</v>
       </c>
       <c r="B410" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" ht="21">
+      <c r="A411" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B411" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C410" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="411" spans="1:3" ht="21">
-      <c r="B411" s="7"/>
-      <c r="C411" s="4"/>
+      <c r="C411" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="B412" s="7"/>
       <c r="C412" s="4"/>
     </row>
     <row r="413" spans="1:3" ht="21">
-      <c r="A413" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="B413" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="C413" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B413" s="7"/>
+      <c r="C413" s="4"/>
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="8" t="s">
         <v>379</v>
       </c>
       <c r="B414" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="21">
@@ -6669,7 +6680,7 @@
         <v>379</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C415" s="4" t="s">
         <v>4</v>
@@ -6680,10 +6691,10 @@
         <v>379</v>
       </c>
       <c r="B416" s="6" t="s">
-        <v>84</v>
+        <v>382</v>
       </c>
       <c r="C416" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="21">
@@ -6691,10 +6702,10 @@
         <v>379</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>383</v>
+        <v>84</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="21">
@@ -6702,37 +6713,37 @@
         <v>379</v>
       </c>
       <c r="B418" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C418" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" ht="21">
+      <c r="A419" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B419" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C418" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="419" spans="1:4" ht="21">
-      <c r="B419" s="7"/>
-      <c r="C419" s="4"/>
+      <c r="C419" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="420" spans="1:4" ht="21">
       <c r="B420" s="7"/>
       <c r="C420" s="4"/>
     </row>
     <row r="421" spans="1:4" ht="21">
-      <c r="A421" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B421" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="C421" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="B421" s="7"/>
+      <c r="C421" s="4"/>
     </row>
     <row r="422" spans="1:4" ht="21">
       <c r="A422" s="5" t="s">
         <v>385</v>
       </c>
       <c r="B422" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>456</v>
@@ -6743,13 +6754,10 @@
         <v>385</v>
       </c>
       <c r="B423" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="D423" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="21">
@@ -6757,10 +6765,13 @@
         <v>385</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C424" s="4" t="s">
         <v>456</v>
+      </c>
+      <c r="D424" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="21">
@@ -6768,7 +6779,7 @@
         <v>385</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>456</v>
@@ -6779,7 +6790,7 @@
         <v>385</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>456</v>
@@ -6790,7 +6801,7 @@
         <v>385</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>456</v>
@@ -6801,7 +6812,7 @@
         <v>385</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>267</v>
+        <v>392</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>456</v>
@@ -6812,7 +6823,7 @@
         <v>385</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>393</v>
+        <v>267</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>456</v>
@@ -6823,7 +6834,7 @@
         <v>385</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>456</v>
@@ -6834,10 +6845,10 @@
         <v>385</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="432" spans="1:4" ht="21">
@@ -6845,10 +6856,10 @@
         <v>385</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>517</v>
+        <v>395</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="21">
@@ -6856,7 +6867,7 @@
         <v>385</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>396</v>
+        <v>517</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>456</v>
@@ -6867,7 +6878,7 @@
         <v>385</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>456</v>
@@ -6878,7 +6889,7 @@
         <v>385</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>456</v>
@@ -6889,7 +6900,7 @@
         <v>385</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>456</v>
@@ -6900,7 +6911,7 @@
         <v>385</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>456</v>
@@ -6911,7 +6922,7 @@
         <v>385</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>456</v>
@@ -6922,7 +6933,7 @@
         <v>385</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>456</v>
@@ -6933,7 +6944,7 @@
         <v>385</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>456</v>
@@ -6944,7 +6955,7 @@
         <v>385</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>456</v>
@@ -6955,7 +6966,7 @@
         <v>385</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>456</v>
@@ -6966,7 +6977,7 @@
         <v>385</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>456</v>
@@ -6977,7 +6988,7 @@
         <v>385</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>456</v>
@@ -6988,7 +6999,7 @@
         <v>385</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>456</v>
@@ -6999,7 +7010,7 @@
         <v>385</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>456</v>
@@ -7010,7 +7021,7 @@
         <v>385</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>456</v>
@@ -7021,7 +7032,7 @@
         <v>385</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>456</v>
@@ -7032,7 +7043,7 @@
         <v>385</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>456</v>
@@ -7043,7 +7054,7 @@
         <v>385</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>456</v>
@@ -7054,7 +7065,7 @@
         <v>385</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>456</v>
@@ -7065,7 +7076,7 @@
         <v>385</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>456</v>
@@ -7076,7 +7087,7 @@
         <v>385</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>456</v>
@@ -7087,7 +7098,7 @@
         <v>385</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>456</v>
@@ -7098,7 +7109,7 @@
         <v>385</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>456</v>
@@ -7109,7 +7120,7 @@
         <v>385</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>456</v>
@@ -7120,7 +7131,7 @@
         <v>385</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>456</v>
@@ -7131,7 +7142,7 @@
         <v>385</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>456</v>
@@ -7142,7 +7153,7 @@
         <v>385</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>456</v>
@@ -7153,7 +7164,7 @@
         <v>385</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>456</v>
@@ -7164,7 +7175,7 @@
         <v>385</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>456</v>
@@ -7175,7 +7186,7 @@
         <v>385</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>456</v>
@@ -7186,7 +7197,7 @@
         <v>385</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>456</v>
@@ -7197,7 +7208,7 @@
         <v>385</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>456</v>
@@ -7208,7 +7219,7 @@
         <v>385</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>456</v>
@@ -7219,7 +7230,7 @@
         <v>385</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>456</v>
@@ -7230,7 +7241,7 @@
         <v>385</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>456</v>
@@ -7241,7 +7252,7 @@
         <v>385</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>456</v>
@@ -7252,7 +7263,7 @@
         <v>385</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>456</v>
@@ -7263,7 +7274,7 @@
         <v>385</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C470" s="4" t="s">
         <v>456</v>
@@ -7274,7 +7285,7 @@
         <v>385</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C471" s="4" t="s">
         <v>456</v>
@@ -7285,10 +7296,10 @@
         <v>385</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>4</v>
+        <v>456</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
@@ -7296,10 +7307,10 @@
         <v>385</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>456</v>
+        <v>4</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
@@ -7307,7 +7318,7 @@
         <v>385</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>456</v>
@@ -7318,7 +7329,7 @@
         <v>385</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>456</v>
@@ -7329,7 +7340,7 @@
         <v>385</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>456</v>
@@ -7340,7 +7351,7 @@
         <v>385</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>456</v>
@@ -7351,7 +7362,7 @@
         <v>385</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>456</v>
@@ -7362,7 +7373,7 @@
         <v>385</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>456</v>
@@ -7373,38 +7384,38 @@
         <v>385</v>
       </c>
       <c r="B480" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C480" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" ht="21">
+      <c r="A481" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B481" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="C480" s="4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" ht="21">
-      <c r="B481" s="7"/>
-      <c r="C481" s="4"/>
+      <c r="C481" s="4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="482" spans="1:3" ht="21">
-      <c r="A482" s="8"/>
       <c r="B482" s="7"/>
       <c r="C482" s="4"/>
     </row>
     <row r="483" spans="1:3" ht="21">
-      <c r="A483" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B483" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="C483" s="4" t="s">
-        <v>456</v>
-      </c>
+      <c r="A483" s="8"/>
+      <c r="B483" s="7"/>
+      <c r="C483" s="4"/>
     </row>
     <row r="484" spans="1:3" ht="21">
       <c r="A484" s="5" t="s">
         <v>444</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C484" s="4" t="s">
         <v>456</v>
@@ -7415,7 +7426,7 @@
         <v>444</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C485" s="4" t="s">
         <v>456</v>
@@ -7426,7 +7437,7 @@
         <v>444</v>
       </c>
       <c r="B486" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C486" s="4" t="s">
         <v>456</v>
@@ -7437,7 +7448,7 @@
         <v>444</v>
       </c>
       <c r="B487" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C487" s="4" t="s">
         <v>456</v>
@@ -7448,7 +7459,7 @@
         <v>444</v>
       </c>
       <c r="B488" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C488" s="4" t="s">
         <v>456</v>
@@ -7459,7 +7470,7 @@
         <v>444</v>
       </c>
       <c r="B489" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C489" s="4" t="s">
         <v>456</v>
@@ -7470,7 +7481,7 @@
         <v>444</v>
       </c>
       <c r="B490" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C490" s="4" t="s">
         <v>456</v>
@@ -7481,7 +7492,7 @@
         <v>444</v>
       </c>
       <c r="B491" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C491" s="4" t="s">
         <v>456</v>
@@ -7492,7 +7503,7 @@
         <v>444</v>
       </c>
       <c r="B492" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C492" s="4" t="s">
         <v>456</v>
@@ -7503,9 +7514,20 @@
         <v>444</v>
       </c>
       <c r="B493" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C493" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" ht="21">
+      <c r="A494" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B494" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="C493" s="4" t="s">
+      <c r="C494" s="4" t="s">
         <v>456</v>
       </c>
     </row>
@@ -7704,268 +7726,268 @@
     <hyperlink ref="B217" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
     <hyperlink ref="B218" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
     <hyperlink ref="B219" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="B223" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="B224" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="B225" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="B226" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="B227" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="B228" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="B229" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="B230" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="B231" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="B232" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="B233" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="B234" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="B235" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="B236" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="B237" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="B238" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="B239" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="B240" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="B241" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="B242" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="B243" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="B244" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="B247" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="B248" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="B249" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="B250" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="B251" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="B253" r:id="rId221" display="Greedy Algorithm to find Minimum number of Coins" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="B254" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="B255" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="B256" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B257" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="B258" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="B259" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="B260" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="B261" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="B262" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="B263" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="B264" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="B265" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="B266" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="B267" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="B268" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="B270" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="B271" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="B272" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="B273" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="B274" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="B275" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="B276" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="B277" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="B278" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="B279" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="B280" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="B281" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="B282" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="B285" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="B286" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="B287" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="B288" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="B289" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="B290" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="B291" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="B292" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="B293" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="B294" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="B295" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="B296" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="B297" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="B298" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="B299" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="B300" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="B301" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="B302" r:id="rId267" display="Partition of a set intoK subsets with equal sum" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="B303" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="B306" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="B307" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="B308" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="B309" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="B310" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="B311" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="B312" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="B313" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="B314" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="B315" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="B316" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="B317" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="B318" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="B319" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="B320" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="B321" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="B322" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="B323" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="B324" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="B325" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="B326" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="B327" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="B328" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="B329" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="B330" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="B331" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="B332" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="B333" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="B334" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="B335" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="B336" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="B337" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="B338" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="B339" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="B340" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="B341" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="B342" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="B343" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="B348" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="B349" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="B350" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="B351" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="B352" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="B353" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="B354" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="B355" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="B356" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="B357" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="B358" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="B359" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="B360" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="B361" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="B362" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="B363" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="B364" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="B365" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="B369" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="B370" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="B371" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="B372" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="B373" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="B374" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="B375" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="B376" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="B377" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="B378" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="B379" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="B380" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="B381" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="B382" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="B383" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="B384" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="B385" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="B386" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="B387" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="B388" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="B389" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="B390" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="B391" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="B392" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="B393" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="B394" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="B395" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="B396" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="B397" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="B398" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="B399" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="B400" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="B401" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="B402" r:id="rId358" display="Find if there is a path of more thank length from a source" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="B403" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="B404" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="B405" r:id="rId361" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="B407" r:id="rId362" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="B406" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="B408" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="B409" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="B410" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="B413" r:id="rId367" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="B414" r:id="rId368" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="B415" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="B416" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="B417" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="B418" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="B421" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="B422" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="B423" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="B424" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="B425" r:id="rId377" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="B426" r:id="rId378" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="B427" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="B428" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="B429" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="B430" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="B431" r:id="rId383" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="B432" r:id="rId384" display="Painting the Fenceproblem" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="B433" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="B434" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="B435" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="B436" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="B437" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="B438" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="B439" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="B440" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="B441" r:id="rId393" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="B442" r:id="rId394" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="B443" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="B444" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="B445" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="B446" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="B447" r:id="rId399" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="B448" r:id="rId400" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="B449" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="B450" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="B451" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="B452" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="B453" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="B454" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="B455" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="B456" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="B457" r:id="rId409" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="B458" r:id="rId410" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="B459" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="B460" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="B462" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="B461" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="B463" r:id="rId415" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="B464" r:id="rId416" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="B465" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="B466" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="B467" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="B468" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="B469" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="B470" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="B471" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="B472" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="B473" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="B480" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="B479" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="B478" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="B477" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="B476" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="B475" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="B474" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="B483" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="B484" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="B485" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="B486" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="B487" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="B488" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="B489" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="B492" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="B490" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="B491" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="B368" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
+    <hyperlink ref="B224" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B225" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="B226" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B227" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="B228" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B229" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="B230" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B231" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="B232" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B233" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="B234" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B235" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="B236" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B237" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="B238" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B239" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="B240" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B241" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="B242" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B243" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="B244" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B245" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B248" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B249" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B250" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B251" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B252" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B254" r:id="rId221" display="Greedy Algorithm to find Minimum number of Coins" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B255" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B256" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B257" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B258" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B259" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B260" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B261" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B262" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B263" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B264" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B265" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B266" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B267" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B268" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B269" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B271" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B272" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B273" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="B274" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B275" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B276" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="B277" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B278" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B279" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B280" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B281" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B282" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B283" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B286" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="B287" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B288" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B289" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B290" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B291" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B292" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B293" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B294" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B295" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B296" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B297" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B298" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B299" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B300" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B301" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B302" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B303" r:id="rId267" display="Partition of a set intoK subsets with equal sum" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B304" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B307" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B308" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B309" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B310" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B311" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B312" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B313" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B314" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B315" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B316" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B317" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B318" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B319" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B320" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B321" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B322" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B323" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B324" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B325" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B326" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B327" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B328" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B329" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B330" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B331" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B332" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B333" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B334" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B335" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B336" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B337" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="B338" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="B339" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="B340" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="B341" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="B342" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="B343" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="B344" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="B349" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="B350" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="B351" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="B352" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="B353" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="B354" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="B355" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B356" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="B357" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="B358" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="B359" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="B360" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="B361" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="B362" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="B363" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="B364" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="B365" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="B366" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="B370" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="B371" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="B372" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="B373" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="B374" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="B375" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="B376" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="B377" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="B378" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="B379" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="B380" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="B381" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="B382" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="B383" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="B384" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="B385" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="B386" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="B387" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="B388" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="B389" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="B390" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="B391" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="B392" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="B393" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="B394" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="B395" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="B396" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="B397" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="B398" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="B399" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="B400" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="B401" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="B402" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="B403" r:id="rId358" display="Find if there is a path of more thank length from a source" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="B404" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="B405" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="B406" r:id="rId361" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="B408" r:id="rId362" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="B407" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="B409" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="B410" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="B411" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="B414" r:id="rId367" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="B415" r:id="rId368" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="B416" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="B417" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="B418" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="B419" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="B422" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="B423" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="B424" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="B425" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="B426" r:id="rId377" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="B427" r:id="rId378" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="B428" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="B429" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="B430" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="B431" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="B432" r:id="rId383" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="B433" r:id="rId384" display="Painting the Fenceproblem" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="B434" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="B435" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="B436" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="B437" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="B438" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="B439" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="B440" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="B441" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="B442" r:id="rId393" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="B443" r:id="rId394" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="B444" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="B445" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="B446" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="B447" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="B448" r:id="rId399" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="B449" r:id="rId400" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="B450" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="B451" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="B452" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="B453" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="B454" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="B455" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="B456" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="B457" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="B458" r:id="rId409" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="B459" r:id="rId410" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="B460" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="B461" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="B463" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="B462" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="B464" r:id="rId415" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="B465" r:id="rId416" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="B466" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="B467" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="B468" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
+    <hyperlink ref="B469" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
+    <hyperlink ref="B470" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
+    <hyperlink ref="B471" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
+    <hyperlink ref="B472" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
+    <hyperlink ref="B473" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
+    <hyperlink ref="B474" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
+    <hyperlink ref="B481" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
+    <hyperlink ref="B480" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
+    <hyperlink ref="B479" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
+    <hyperlink ref="B478" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
+    <hyperlink ref="B477" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
+    <hyperlink ref="B476" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
+    <hyperlink ref="B475" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
+    <hyperlink ref="B484" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
+    <hyperlink ref="B485" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
+    <hyperlink ref="B486" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
+    <hyperlink ref="B487" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
+    <hyperlink ref="B488" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
+    <hyperlink ref="B489" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
+    <hyperlink ref="B490" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
+    <hyperlink ref="B493" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
+    <hyperlink ref="B491" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
+    <hyperlink ref="B492" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
+    <hyperlink ref="B369" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
     <hyperlink ref="B2" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
     <hyperlink ref="B42" r:id="rId445" location=":~:text=Determine%20if%20array%20A%20can,%5D)%2C%20otherwise%20print%20%2D1." xr:uid="{00000000-0004-0000-0000-0000BE010000}"/>
     <hyperlink ref="B87" r:id="rId446" display="first repeated word in a string" xr:uid="{00000000-0004-0000-0000-0000BF010000}"/>
     <hyperlink ref="B141" r:id="rId447" xr:uid="{00000000-0004-0000-0000-0000C0010000}"/>
     <hyperlink ref="B170" r:id="rId448" location=":~:text=Why%20is%20Merge%20Sort%20preferred%20for%20Linked%20Lists%3F&amp;text=Unlike%20array%2C%20in%20linked%20list,extra%20space%20for%20linked%20lists." xr:uid="{00000000-0004-0000-0000-0000C1010000}"/>
-    <hyperlink ref="B493" r:id="rId449" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
+    <hyperlink ref="B494" r:id="rId449" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
     <hyperlink ref="B43" r:id="rId450" xr:uid="{00000000-0004-0000-0000-0000C3010000}"/>
-    <hyperlink ref="B344" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
+    <hyperlink ref="B345" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
     <hyperlink ref="B182" r:id="rId452" xr:uid="{B0973ED4-D13A-4CAC-AE75-C246475B5543}"/>
     <hyperlink ref="B183" r:id="rId453" xr:uid="{5967A2A7-F68E-43A1-B930-C9AB00BA0A7F}"/>
-    <hyperlink ref="B252" r:id="rId454" display="Number Of Coin" xr:uid="{85C57855-7A7E-49C4-8262-64308D8D2582}"/>
-    <hyperlink ref="B269" r:id="rId455" xr:uid="{394D666A-9661-42D1-9B3B-C374DE0102E0}"/>
+    <hyperlink ref="B253" r:id="rId454" display="Number Of Coin" xr:uid="{85C57855-7A7E-49C4-8262-64308D8D2582}"/>
+    <hyperlink ref="B270" r:id="rId455" xr:uid="{394D666A-9661-42D1-9B3B-C374DE0102E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId456"/>

</xml_diff>